<commit_message>
Fixed: excel error; Added: category name editing
</commit_message>
<xml_diff>
--- a/media/basedata/innopolis_lyceum_participants.xlsx
+++ b/media/basedata/innopolis_lyceum_participants.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t>никита</t>
   </si>
@@ -30,6 +30,15 @@
   </si>
   <si>
     <t>participant_6</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>sad</t>
+  </si>
+  <si>
+    <t>participant_19</t>
   </si>
 </sst>
 </file>
@@ -371,7 +380,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -397,6 +406,26 @@
       </c>
       <c r="F2">
         <v>4873176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>6615829</v>
       </c>
     </row>
   </sheetData>

</xml_diff>